<commit_message>
parametri per singolo comune
</commit_message>
<xml_diff>
--- a/scenari/BO_soli.xlsx
+++ b/scenari/BO_soli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\forna\Repos\elezioni\scenari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626E2D0E-2A2B-4539-808E-3B93AF56CAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC36E76-7FFE-4C0D-BBA1-204FF1EEF419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="108">
   <si>
     <t>LISTA_FUTURA</t>
   </si>
@@ -438,8 +438,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25CD1B6C-5176-4636-A295-76158BC84BCA}" name="Tabella1" displayName="Tabella1" ref="A1:E104" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:E104" xr:uid="{25CD1B6C-5176-4636-A295-76158BC84BCA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25CD1B6C-5176-4636-A295-76158BC84BCA}" name="Tabella1" displayName="Tabella1" ref="A1:E103" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:E103" xr:uid="{25CD1B6C-5176-4636-A295-76158BC84BCA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{44211973-D4BF-4489-936E-2C4681187FB6}" name="DATA" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{77E90632-A809-40F6-8A9A-D84A288AB0B0}" name="ELEZIONE"/>
@@ -884,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E96" sqref="E96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2436,11 +2436,14 @@
       <c r="B91" t="s">
         <v>72</v>
       </c>
+      <c r="C91" t="s">
+        <v>73</v>
+      </c>
       <c r="D91" t="s">
-        <v>25</v>
+        <v>105</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -2454,10 +2457,10 @@
         <v>73</v>
       </c>
       <c r="D92" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E92">
-        <v>0.38</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -2468,13 +2471,13 @@
         <v>72</v>
       </c>
       <c r="C93" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D93" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="E93">
-        <v>0.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -2485,10 +2488,10 @@
         <v>72</v>
       </c>
       <c r="C94" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D94" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -2502,10 +2505,10 @@
         <v>72</v>
       </c>
       <c r="C95" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D95" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -2519,10 +2522,10 @@
         <v>72</v>
       </c>
       <c r="C96" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -2536,10 +2539,10 @@
         <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D97" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -2553,10 +2556,10 @@
         <v>72</v>
       </c>
       <c r="C98" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D98" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -2570,10 +2573,10 @@
         <v>72</v>
       </c>
       <c r="C99" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D99" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2587,10 +2590,10 @@
         <v>72</v>
       </c>
       <c r="C100" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="D100" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -2604,10 +2607,10 @@
         <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D101" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2621,10 +2624,10 @@
         <v>72</v>
       </c>
       <c r="C102" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D102" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -2638,29 +2641,12 @@
         <v>72</v>
       </c>
       <c r="C103" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="D103" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="E103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="2">
-        <v>45612.958333333328</v>
-      </c>
-      <c r="B104" t="s">
-        <v>72</v>
-      </c>
-      <c r="C104" t="s">
-        <v>25</v>
-      </c>
-      <c r="D104" t="s">
-        <v>25</v>
-      </c>
-      <c r="E104">
         <v>1</v>
       </c>
     </row>
@@ -2676,7 +2662,7 @@
           <x14:formula1>
             <xm:f>liste_future!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D104</xm:sqref>
+          <xm:sqref>D2:D103</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>